<commit_message>
fixes on XLSX and config
</commit_message>
<xml_diff>
--- a/tests/data/mendeley_testing_dataset.xlsx
+++ b/tests/data/mendeley_testing_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\PII Model\Final_Model\Python Script Testing\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry.delprat/dev/scruby/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23F3C4-3625-4765-880D-C9A64DED2BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBF2FAB-3CF2-F840-8560-5346191BCC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF101000-2A9D-4C13-ADDC-FAADCDA255BE}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="23260" windowHeight="12460" xr2:uid="{FF101000-2A9D-4C13-ADDC-FAADCDA255BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing_Set" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="299">
   <si>
     <t>Name</t>
   </si>
@@ -157,13 +157,6 @@
   </si>
   <si>
     <t>Jonathon Roth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maestro
-April West
-503881435914 08/34
-CVV: 862
-</t>
   </si>
   <si>
     <t>gordonlisa@example.net</t>
@@ -330,9 +323,6 @@
     <t>https://larson.com/</t>
   </si>
   <si>
-    <t>+95 5309404752</t>
-  </si>
-  <si>
     <t>18056 Gregory Well Suite 659
 East Aliciashire, NE 90956</t>
   </si>
@@ -363,9 +353,6 @@
   </si>
   <si>
     <t>http://rodgers.com/</t>
-  </si>
-  <si>
-    <t>+56 8366018544</t>
   </si>
   <si>
     <t>714 Kane Forks Apt. 893
@@ -412,9 +399,6 @@
   </si>
   <si>
     <t>http://www.crawford-cuevas.com/</t>
-  </si>
-  <si>
-    <t>+65 9282270124</t>
   </si>
   <si>
     <t>1831 Ashley Mountains Suite 943
@@ -556,9 +540,6 @@
     <t>http://wilkinson.com/</t>
   </si>
   <si>
-    <t>+211 9612363682</t>
-  </si>
-  <si>
     <t>75395 Anthony Pines
 South April, TX 37507</t>
   </si>
@@ -676,9 +657,6 @@
     <t>http://white.org/</t>
   </si>
   <si>
-    <t>+68 7123796774</t>
-  </si>
-  <si>
     <t>USNS Orr
 FPO AA 39270</t>
   </si>
@@ -796,9 +774,6 @@
     <t>https://mann.com/</t>
   </si>
   <si>
-    <t>+641 9362489101</t>
-  </si>
-  <si>
     <t>07808 Matthews Estates
 South Josephbury, PW 36341</t>
   </si>
@@ -834,9 +809,6 @@
   </si>
   <si>
     <t>http://www.johnson.com/</t>
-  </si>
-  <si>
-    <t>+126 5405174108</t>
   </si>
   <si>
     <t>94967 Vasquez Skyway
@@ -921,9 +893,6 @@
     <t>https://rios-santiago.com/</t>
   </si>
   <si>
-    <t>+318 8989212289</t>
-  </si>
-  <si>
     <t>Unit 4795 Box 2012
 DPO AA 70258</t>
   </si>
@@ -961,9 +930,6 @@
     <t>http://mendoza.com/</t>
   </si>
   <si>
-    <t>+30 3873936001</t>
-  </si>
-  <si>
     <t>1534 Monica Union Suite 648
 Lake Erinland, IA 16557</t>
   </si>
@@ -1239,9 +1205,6 @@
   </si>
   <si>
     <t>https://proctor-wright.biz/</t>
-  </si>
-  <si>
-    <t>+05 9476402241</t>
   </si>
   <si>
     <t>6917 Alicia Lakes Suite 176
@@ -1902,9 +1865,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1942,7 +1905,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2048,7 +2011,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2190,7 +2153,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2200,25 +2163,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF73E6B-4B81-432E-9C77-B79E7D992B8A}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="15" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="37.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="35.21875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="37.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="35.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +2245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2314,903 +2277,882 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="1" t="s">
+    <row r="6" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="1" t="s">
+    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="1" t="s">
+    <row r="8" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="2" t="s">
+    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="2" t="s">
+    <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="2" t="s">
+    <row r="11" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="2" t="s">
+    <row r="12" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" s="2" t="s">
+    <row r="13" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="2" t="s">
+    <row r="14" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="F14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" s="2" t="s">
+    <row r="15" spans="1:10" ht="240" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="2" t="s">
+    <row r="16" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="2" t="s">
+    <row r="17" spans="1:10" ht="288" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="G17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E17" s="2" t="s">
+    <row r="18" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="H18" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D18" s="2" t="s">
+    <row r="19" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="H19" s="2" t="s">
         <v>179</v>
       </c>
+      <c r="I19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C19" s="2" t="s">
+    <row r="20" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="H20" s="2" t="s">
         <v>189</v>
       </c>
+      <c r="I20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C20" s="2" t="s">
+    <row r="21" spans="1:10" ht="240" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="H21" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="J21" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B21" s="2" t="s">
+    <row r="22" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="288" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:10" ht="240" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I29" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J28" s="1" t="s">
+    </row>
+    <row r="30" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="29" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="J29" s="1" t="s">
+    <row r="31" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I31" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>